<commit_message>
60minute yaml file run
</commit_message>
<xml_diff>
--- a/two_line_alerts_60minute.xlsx
+++ b/two_line_alerts_60minute.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M2047"/>
+  <dimension ref="A1:M2050"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -92574,6 +92574,141 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2048">
+      <c r="A2048" t="inlineStr">
+        <is>
+          <t>NIFTY BANK</t>
+        </is>
+      </c>
+      <c r="B2048" s="2" t="n">
+        <v>44942.42708333334</v>
+      </c>
+      <c r="C2048" t="n">
+        <v>71</v>
+      </c>
+      <c r="D2048" s="2" t="n">
+        <v>44932.59375</v>
+      </c>
+      <c r="E2048" t="n">
+        <v>33</v>
+      </c>
+      <c r="F2048" t="n">
+        <v>41881.45</v>
+      </c>
+      <c r="G2048" s="2" t="n">
+        <v>44938.55208333334</v>
+      </c>
+      <c r="H2048" t="n">
+        <v>60</v>
+      </c>
+      <c r="I2048" t="n">
+        <v>41746.3</v>
+      </c>
+      <c r="J2048" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="K2048" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2048" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2048" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2049">
+      <c r="A2049" t="inlineStr">
+        <is>
+          <t>NIFTY FIN SERVICE</t>
+        </is>
+      </c>
+      <c r="B2049" s="2" t="n">
+        <v>45202.51041666666</v>
+      </c>
+      <c r="C2049" t="n">
+        <v>1298</v>
+      </c>
+      <c r="D2049" s="2" t="n">
+        <v>45191.59375</v>
+      </c>
+      <c r="E2049" t="n">
+        <v>1258</v>
+      </c>
+      <c r="F2049" t="n">
+        <v>19708.1</v>
+      </c>
+      <c r="G2049" s="2" t="n">
+        <v>45197.63541666666</v>
+      </c>
+      <c r="H2049" t="n">
+        <v>1287</v>
+      </c>
+      <c r="I2049" t="n">
+        <v>19649.35</v>
+      </c>
+      <c r="J2049" t="inlineStr">
+        <is>
+          <t>Low</t>
+        </is>
+      </c>
+      <c r="K2049" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2049" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2049" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2050">
+      <c r="A2050" t="inlineStr">
+        <is>
+          <t>NIFTY FIN SERVICE</t>
+        </is>
+      </c>
+      <c r="B2050" s="2" t="n">
+        <v>45289.55208333334</v>
+      </c>
+      <c r="C2050" t="n">
+        <v>1713</v>
+      </c>
+      <c r="D2050" s="2" t="n">
+        <v>45280.38541666666</v>
+      </c>
+      <c r="E2050" t="n">
+        <v>1667</v>
+      </c>
+      <c r="F2050" t="n">
+        <v>21552.35</v>
+      </c>
+      <c r="G2050" s="2" t="n">
+        <v>45288.38541666666</v>
+      </c>
+      <c r="H2050" t="n">
+        <v>1702</v>
+      </c>
+      <c r="I2050" t="n">
+        <v>21627.35</v>
+      </c>
+      <c r="J2050" t="inlineStr">
+        <is>
+          <t>High</t>
+        </is>
+      </c>
+      <c r="K2050" t="n">
+        <v>10</v>
+      </c>
+      <c r="L2050" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2050" t="n">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>